<commit_message>
enable logging in the multibeggar project [close #2]
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_portfolio_complexity_data.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_portfolio_complexity_data.xlsx
@@ -534,7 +534,7 @@
         <v>43826</v>
       </c>
       <c r="C9" t="n">
-        <v>1.011122405604997</v>
+        <v>1.013382075887503</v>
       </c>
     </row>
     <row r="10">
@@ -545,7 +545,7 @@
         <v>43836</v>
       </c>
       <c r="C10" t="n">
-        <v>1.012411187578234</v>
+        <v>1.021144200595874</v>
       </c>
     </row>
     <row r="11">
@@ -556,7 +556,7 @@
         <v>43844</v>
       </c>
       <c r="C11" t="n">
-        <v>1.012185968318799</v>
+        <v>1.020265187051211</v>
       </c>
     </row>
     <row r="12">
@@ -567,7 +567,7 @@
         <v>43851</v>
       </c>
       <c r="C12" t="n">
-        <v>1.012756569864679</v>
+        <v>1.020136396917592</v>
       </c>
     </row>
     <row r="13">
@@ -578,7 +578,7 @@
         <v>43858</v>
       </c>
       <c r="C13" t="n">
-        <v>1.013209336252091</v>
+        <v>1.020421219193817</v>
       </c>
     </row>
     <row r="14">
@@ -589,7 +589,7 @@
         <v>43862</v>
       </c>
       <c r="C14" t="n">
-        <v>1.008126650968759</v>
+        <v>1.014783377783833</v>
       </c>
     </row>
     <row r="15">
@@ -600,7 +600,7 @@
         <v>43868</v>
       </c>
       <c r="C15" t="n">
-        <v>1.009593702999345</v>
+        <v>1.023577558129962</v>
       </c>
     </row>
     <row r="16">
@@ -611,7 +611,7 @@
         <v>43871</v>
       </c>
       <c r="C16" t="n">
-        <v>1.01159787454516</v>
+        <v>1.021533795909439</v>
       </c>
     </row>
     <row r="17">
@@ -622,7 +622,7 @@
         <v>43878</v>
       </c>
       <c r="C17" t="n">
-        <v>1.011957735177982</v>
+        <v>1.023089942607398</v>
       </c>
     </row>
     <row r="18">
@@ -633,7 +633,7 @@
         <v>43894</v>
       </c>
       <c r="C18" t="n">
-        <v>1.013299035341718</v>
+        <v>1.02318315857201</v>
       </c>
     </row>
     <row r="19">
@@ -644,7 +644,7 @@
         <v>43909</v>
       </c>
       <c r="C19" t="n">
-        <v>1.012432740525532</v>
+        <v>1.024902458094388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>